<commit_message>
modifications mineures du Excell, création basique de tous les métas characters et amélioration du BaseCharacter
</commit_message>
<xml_diff>
--- a/Assets/Ressources/GameJam.xlsx
+++ b/Assets/Ressources/GameJam.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JeremyBouchard/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\GameJamA2016\Assets\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="6020" windowWidth="28720" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="10440" yWindow="6015" windowWidth="28725" windowHeight="17595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Artiste</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Hack</t>
   </si>
   <si>
-    <t>Besoin someil</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -93,12 +90,18 @@
   </si>
   <si>
     <t>1+0.1*Stat_En_Art</t>
+  </si>
+  <si>
+    <t>Sleep Resist</t>
+  </si>
+  <si>
+    <t>Attack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,8 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,6 +145,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -409,31 +418,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="32.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -443,14 +453,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -460,16 +470,16 @@
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>5</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -477,16 +487,16 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -494,14 +504,14 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>5</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" ref="B6:C6" si="0">SUM(B2:B4)</f>
         <v>16</v>
@@ -510,7 +520,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f>SUM(D2:D4)</f>
         <v>16</v>
       </c>
@@ -519,74 +529,74 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>